<commit_message>
Removed teh burden analysis portion into different project
</commit_message>
<xml_diff>
--- a/Results/Tables/Asthma_years.xlsx
+++ b/Results/Tables/Asthma_years.xlsx
@@ -17,19 +17,19 @@
     <t>State</t>
   </si>
   <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>2007</t>
+  </si>
+  <si>
+    <t>2008</t>
+  </si>
+  <si>
+    <t>2009</t>
+  </si>
+  <si>
+    <t>2010</t>
   </si>
   <si>
     <t>Aggregate</t>

</xml_diff>